<commit_message>
working on spatial diffusion - realising that a max criteria needs to be defined otherwise certain regions more than 100
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="18255" windowHeight="11310"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18255" windowHeight="11250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,6 +287,80 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>703384</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>315058</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7964365" y="3436327"/>
+          <a:ext cx="2329962" cy="915865"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Attention:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> Like this, if high values are choosen certain regions can have more than 100% diffusion. A solution might be to define a max criteria. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,7 +653,7 @@
   <dimension ref="C2:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="I18" sqref="I18:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="1">
-        <v>0.4</v>
+        <v>0.9</v>
       </c>
       <c r="N4" t="s">
         <v>7</v>
@@ -629,7 +703,7 @@
       </c>
       <c r="J5" s="2">
         <f>G8*J4</f>
-        <v>1200</v>
+        <v>2700</v>
       </c>
       <c r="N5" t="s">
         <v>9</v>
@@ -776,7 +850,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -794,27 +868,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="3"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>22</v>
       </c>
       <c r="E20">
         <f>J5*E17</f>
-        <v>290.90909090909093</v>
+        <v>654.54545454545462</v>
       </c>
       <c r="F20">
         <f>J5*F17</f>
-        <v>909.09090909090912</v>
+        <v>2045.4545454545455</v>
       </c>
       <c r="G20" s="2">
         <f>E20+F20</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2700</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>23</v>
       </c>
@@ -830,39 +912,41 @@
         <f>E21+F21</f>
         <v>1800</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E22">
         <f>E21+E20</f>
-        <v>727.27272727272737</v>
+        <v>1090.909090909091</v>
       </c>
       <c r="F22">
         <f>F21+F20</f>
-        <v>2272.7272727272725</v>
+        <v>3409.090909090909</v>
       </c>
       <c r="G22">
         <f>E22+F22</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>27</v>
       </c>
       <c r="E24">
         <f>E20/E8</f>
-        <v>0.29090909090909095</v>
+        <v>0.65454545454545465</v>
       </c>
       <c r="F24">
         <f>F20/F8</f>
-        <v>0.45454545454545459</v>
+        <v>1.0227272727272727</v>
       </c>
       <c r="G24">
         <f>SUM(E24:F24)</f>
-        <v>0.74545454545454559</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+        <v>1.6772727272727272</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>28</v>
       </c>
@@ -879,16 +963,16 @@
         <v>1.1181818181818182</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>29</v>
       </c>
       <c r="I26" s="2">
         <f>E24*E8+F24*F8</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>30</v>
       </c>
@@ -900,6 +984,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implemented that population density is used to differentiated diffusion speed
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="18255" windowHeight="11190"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="18255" windowHeight="2745" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="only_speed" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>A</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>v</t>
+  </si>
+  <si>
+    <t>fator to reduce</t>
+  </si>
+  <si>
+    <t>faktor to reduce with normed</t>
+  </si>
+  <si>
+    <t>TEST NEW FOR A SINGLE FACTOR</t>
+  </si>
+  <si>
+    <t>YJUPI</t>
   </si>
 </sst>
 </file>
@@ -736,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
@@ -1122,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O27"/>
+  <dimension ref="C2:O35"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D27" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="1">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="N4" t="s">
         <v>7</v>
@@ -1175,7 +1187,7 @@
       </c>
       <c r="J5" s="2">
         <f>G8*J4</f>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="N5" t="s">
         <v>9</v>
@@ -1213,7 +1225,7 @@
         <v>6</v>
       </c>
       <c r="J7" s="1">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
@@ -1237,7 +1249,7 @@
       </c>
       <c r="J8" s="2">
         <f>G8*J7</f>
-        <v>1800</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
@@ -1316,10 +1328,6 @@
       <c r="G15">
         <f>E15+F15</f>
         <v>1.0000000000000002</v>
-      </c>
-      <c r="J15">
-        <f>E14/F14</f>
-        <v>0.64</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
@@ -1355,15 +1363,15 @@
       </c>
       <c r="E20">
         <f>J5*E17</f>
-        <v>654.54545454545462</v>
+        <v>290.90909090909093</v>
       </c>
       <c r="F20">
         <f>J5*F17</f>
-        <v>2045.4545454545455</v>
+        <v>909.09090909090912</v>
       </c>
       <c r="G20" s="2">
         <f>E20+F20</f>
-        <v>2700</v>
+        <v>1200</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -1374,15 +1382,15 @@
       </c>
       <c r="E21">
         <f>J8*E17</f>
-        <v>436.36363636363643</v>
+        <v>363.63636363636368</v>
       </c>
       <c r="F21">
         <f>J8*F17</f>
-        <v>1363.6363636363635</v>
+        <v>1136.3636363636363</v>
       </c>
       <c r="G21" s="2">
         <f>E21+F21</f>
-        <v>1800</v>
+        <v>1500</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -1390,15 +1398,15 @@
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E22">
         <f>E21+E20</f>
-        <v>1090.909090909091</v>
+        <v>654.54545454545462</v>
       </c>
       <c r="F22">
         <f>F21+F20</f>
-        <v>3409.090909090909</v>
+        <v>2045.4545454545455</v>
       </c>
       <c r="G22">
         <f>E22+F22</f>
-        <v>4500</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
@@ -1407,15 +1415,15 @@
       </c>
       <c r="E24">
         <f>E20/E8</f>
-        <v>0.65454545454545465</v>
+        <v>0.29090909090909095</v>
       </c>
       <c r="F24">
         <f>F20/F8</f>
-        <v>1.0227272727272727</v>
+        <v>0.45454545454545459</v>
       </c>
       <c r="G24">
         <f>SUM(E24:F24)</f>
-        <v>1.6772727272727272</v>
+        <v>0.74545454545454559</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
@@ -1424,15 +1432,15 @@
       </c>
       <c r="E25">
         <f>E21/E8</f>
-        <v>0.43636363636363645</v>
+        <v>0.3636363636363637</v>
       </c>
       <c r="F25">
         <f>F21/F8</f>
-        <v>0.68181818181818177</v>
+        <v>0.56818181818181812</v>
       </c>
       <c r="G25">
         <f>SUM(E25:F25)</f>
-        <v>1.1181818181818182</v>
+        <v>0.93181818181818188</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
@@ -1441,7 +1449,7 @@
       </c>
       <c r="I26" s="2">
         <f>E24*E8+F24*F8</f>
-        <v>2700</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
@@ -1450,7 +1458,54 @@
       </c>
       <c r="I27" s="2">
         <f>E25*E8+F25*F8</f>
-        <v>1800</v>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <f>D32*E17</f>
+        <v>0.12121212121212123</v>
+      </c>
+      <c r="F32">
+        <f>D32*F17</f>
+        <v>0.37878787878787878</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33">
+        <f>(D32*E17)/E7</f>
+        <v>0.3636363636363637</v>
+      </c>
+      <c r="F33">
+        <f>(D32*F17)/F7</f>
+        <v>0.56818181818181823</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35">
+        <f>(E14/F14) *D32</f>
+        <v>0.32</v>
+      </c>
+      <c r="F35">
+        <f>(F14/F14) *D32</f>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding sim param to assumptions
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -1136,8 +1136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,15 +1471,15 @@
         <v>35</v>
       </c>
       <c r="D32">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <f>D32*E17</f>
-        <v>0.12121212121212123</v>
+        <v>0.24242424242424246</v>
       </c>
       <c r="F32">
         <f>D32*F17</f>
-        <v>0.37878787878787878</v>
+        <v>0.75757575757575757</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
@@ -1488,11 +1488,11 @@
       </c>
       <c r="E33">
         <f>(D32*E17)/E7</f>
-        <v>0.3636363636363637</v>
+        <v>0.7272727272727274</v>
       </c>
       <c r="F33">
         <f>(D32*F17)/F7</f>
-        <v>0.56818181818181823</v>
+        <v>1.1363636363636365</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -1501,11 +1501,11 @@
       </c>
       <c r="E35">
         <f>(E14/F14) *D32</f>
-        <v>0.32</v>
+        <v>0.64</v>
       </c>
       <c r="F35">
         <f>(F14/F14) *D32</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added temps in object
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -127,13 +127,25 @@
     <t>fator to reduce</t>
   </si>
   <si>
-    <t>faktor to reduce with normed</t>
-  </si>
-  <si>
     <t>TEST NEW FOR A SINGLE FACTOR</t>
   </si>
   <si>
-    <t>YJUPI</t>
+    <t>var reg</t>
+  </si>
+  <si>
+    <t>faktor to reduce with normed varreg</t>
+  </si>
+  <si>
+    <t>f_reg_not_normalised</t>
+  </si>
+  <si>
+    <t>f_reg_normalised</t>
+  </si>
+  <si>
+    <t>factor_not_normalised</t>
+  </si>
+  <si>
+    <t>factor_normalised</t>
   </si>
 </sst>
 </file>
@@ -149,7 +161,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +195,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -297,6 +333,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O35"/>
+  <dimension ref="C2:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,51 +1501,113 @@
         <v>1500</v>
       </c>
     </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+    </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="C31" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="20">
+        <v>4</v>
+      </c>
+      <c r="E31" s="17">
+        <f>D31*E17</f>
+        <v>0.96969696969696983</v>
+      </c>
+      <c r="F31" s="17">
+        <f>D31*F17</f>
+        <v>3.0303030303030303</v>
+      </c>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17">
+        <f>(D31*E17)/E7</f>
+        <v>2.9090909090909096</v>
+      </c>
+      <c r="F32" s="17">
+        <f>(D31*F17)/F7</f>
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18">
+        <f>(E37)/((E37*E7+F37*F7))*D31</f>
+        <v>2.9090909090909096</v>
+      </c>
+      <c r="F34" s="18">
+        <f>(F14) / (E7*E14+F7*F14)*D31</f>
+        <v>4.5454545454545459</v>
+      </c>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19">
+        <f>(E37)/((E37*E7+F37*F7))</f>
+        <v>0.7272727272727274</v>
+      </c>
+      <c r="F35" s="19">
+        <f>(F14)/(E7*E14+F7*F14)</f>
+        <v>1.1363636363636365</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18">
+        <f>(E14/F14) *D31</f>
+        <v>2.56</v>
+      </c>
+      <c r="F36" s="18">
+        <f>(F14) / (E7*E14+F7*F14)</f>
+        <v>1.1363636363636365</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19">
+        <f>(E14/F14)</f>
+        <v>0.64</v>
+      </c>
+      <c r="F37" s="19">
+        <f>(F14/F14)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <f>D32*E17</f>
-        <v>0.24242424242424246</v>
-      </c>
-      <c r="F32">
-        <f>D32*F17</f>
-        <v>0.75757575757575757</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33">
-        <f>(D32*E17)/E7</f>
-        <v>0.7272727272727274</v>
-      </c>
-      <c r="F33">
-        <f>(D32*F17)/F7</f>
-        <v>1.1363636363636365</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35">
-        <f>(E14/F14) *D32</f>
-        <v>0.64</v>
-      </c>
-      <c r="F35">
-        <f>(F14/F14) *D32</f>
-        <v>1</v>
+      <c r="E39">
+        <f>(E36)/((E36*E7+F36*F7))*D31</f>
+        <v>6.3566591422121901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactured diffusion value calculation
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>A</t>
   </si>
@@ -130,9 +130,6 @@
     <t>TEST NEW FOR A SINGLE FACTOR</t>
   </si>
   <si>
-    <t>var reg</t>
-  </si>
-  <si>
     <t>faktor to reduce with normed varreg</t>
   </si>
   <si>
@@ -146,6 +143,12 @@
   </si>
   <si>
     <t>factor_normalised</t>
+  </si>
+  <si>
+    <t>factor_reg_norm_abs</t>
+  </si>
+  <si>
+    <t>f_reg_norm_abs</t>
   </si>
 </sst>
 </file>
@@ -206,19 +209,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1174,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:O39"/>
+  <dimension ref="C2:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,7 +1516,7 @@
       <c r="C31" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="18">
         <v>4</v>
       </c>
       <c r="E31" s="17">
@@ -1524,11 +1527,11 @@
         <f>D31*F17</f>
         <v>3.0303030303030303</v>
       </c>
-      <c r="G31" s="17"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C32" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17">
@@ -1539,76 +1542,112 @@
         <f>(D31*F17)/F7</f>
         <v>4.5454545454545459</v>
       </c>
-      <c r="G32" s="17"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="17"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19">
+        <f>E35 *D31</f>
+        <v>2.56</v>
+      </c>
+      <c r="F34" s="19">
+        <f>D31*F35</f>
+        <v>4</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" ref="G34:G38" si="0">SUM(E34:F34)</f>
+        <v>6.5600000000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18">
-        <f>(E37)/((E37*E7+F37*F7))*D31</f>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20">
+        <f>(E14/F14)</f>
+        <v>0.64</v>
+      </c>
+      <c r="F35" s="20">
+        <f>(F14/F14)</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19">
+        <f>E37*D31</f>
         <v>2.9090909090909096</v>
       </c>
-      <c r="F34" s="18">
-        <f>(F14) / (E7*E14+F7*F14)*D31</f>
+      <c r="F36" s="19">
+        <f>D31*F37</f>
         <v>4.5454545454545459</v>
       </c>
-      <c r="G34" s="17"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19">
-        <f>(E37)/((E37*E7+F37*F7))</f>
+      <c r="G36" s="3">
+        <f t="shared" si="0"/>
+        <v>7.454545454545455</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20">
+        <f>(E35)/(E35*E7+F35*F7)</f>
         <v>0.7272727272727274</v>
       </c>
-      <c r="F35" s="19">
+      <c r="F37" s="20">
         <f>(F14)/(E7*E14+F7*F14)</f>
         <v>1.1363636363636365</v>
       </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18">
-        <f>(E14/F14) *D31</f>
-        <v>2.56</v>
-      </c>
-      <c r="F36" s="18">
-        <f>(F14) / (E7*E14+F7*F14)</f>
-        <v>1.1363636363636365</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19">
-        <f>(E14/F14)</f>
-        <v>0.64</v>
-      </c>
-      <c r="F37" s="19">
-        <f>(F14/F14)</f>
-        <v>1</v>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19">
+        <f>D31*E39</f>
+        <v>1.5609756097560974</v>
+      </c>
+      <c r="F38" s="19">
+        <f>D31*F39</f>
+        <v>2.4390243902439024</v>
+      </c>
+      <c r="G38" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E39">
-        <f>(E36)/((E36*E7+F36*F7))*D31</f>
-        <v>6.3566591422121901</v>
-      </c>
+      <c r="C39" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20">
+        <f>E35/(E35+F35)</f>
+        <v>0.39024390243902435</v>
+      </c>
+      <c r="F39" s="20">
+        <f>F35/(E35+F35)</f>
+        <v>0.6097560975609756</v>
+      </c>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
making service switches regional
</commit_message>
<xml_diff>
--- a/config_data/02-spatial_index/spatial_index_example.xlsx
+++ b/config_data/02-spatial_index/spatial_index_example.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>A</t>
   </si>
@@ -133,22 +133,19 @@
     <t>faktor to reduce with normed varreg</t>
   </si>
   <si>
-    <t>f_reg_not_normalised</t>
-  </si>
-  <si>
-    <t>f_reg_normalised</t>
-  </si>
-  <si>
-    <t>factor_not_normalised</t>
-  </si>
-  <si>
-    <t>factor_normalised</t>
-  </si>
-  <si>
-    <t>factor_reg_norm_abs</t>
-  </si>
-  <si>
     <t>f_reg_norm_abs</t>
+  </si>
+  <si>
+    <t>f_reg</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>f_reg_norm</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1177,7 @@
   <dimension ref="C2:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,15 +1514,15 @@
         <v>35</v>
       </c>
       <c r="D31" s="18">
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="E31" s="17">
         <f>D31*E17</f>
-        <v>0.96969696969696983</v>
+        <v>4.8484848484848492E-2</v>
       </c>
       <c r="F31" s="17">
         <f>D31*F17</f>
-        <v>3.0303030303030303</v>
+        <v>0.15151515151515152</v>
       </c>
       <c r="G31" s="3"/>
     </row>
@@ -1536,11 +1533,11 @@
       <c r="D32" s="17"/>
       <c r="E32" s="17">
         <f>(D31*E17)/E7</f>
-        <v>2.9090909090909096</v>
+        <v>0.14545454545454548</v>
       </c>
       <c r="F32" s="17">
         <f>(D31*F17)/F7</f>
-        <v>4.5454545454545459</v>
+        <v>0.22727272727272729</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -1549,20 +1546,20 @@
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19">
         <f>E35 *D31</f>
-        <v>2.56</v>
+        <v>0.128</v>
       </c>
       <c r="F34" s="19">
         <f>D31*F35</f>
-        <v>4</v>
+        <v>0.2</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" ref="G34:G38" si="0">SUM(E34:F34)</f>
-        <v>6.5600000000000005</v>
+        <v>0.32800000000000001</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
@@ -1582,25 +1579,25 @@
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19">
         <f>E37*D31</f>
-        <v>2.9090909090909096</v>
+        <v>0.14545454545454548</v>
       </c>
       <c r="F36" s="19">
         <f>D31*F37</f>
-        <v>4.5454545454545459</v>
+        <v>0.22727272727272729</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="0"/>
-        <v>7.454545454545455</v>
+        <v>0.3727272727272728</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20">
@@ -1615,20 +1612,20 @@
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="19" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19">
         <f>D31*E39</f>
-        <v>1.5609756097560974</v>
+        <v>7.8048780487804878E-2</v>
       </c>
       <c r="F38" s="19">
         <f>D31*F39</f>
-        <v>2.4390243902439024</v>
+        <v>0.12195121951219512</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>